<commit_message>
API sheet for the project created
</commit_message>
<xml_diff>
--- a/04_API/APIs.xlsx
+++ b/04_API/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\github-for-aspire\capstone\04_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6070977E-D667-4675-87D6-D31FB685B84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8602A2AE-3855-451D-86F1-F01AEB605DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>Sr No</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>404: No posts</t>
-  </si>
-  <si>
-    <t>AUTH / USER related APIS:</t>
   </si>
   <si>
     <t>/auth/register</t>
@@ -525,14 +522,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="54.109375" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" customWidth="1"/>
     <col min="5" max="5" width="28.6640625" customWidth="1"/>
     <col min="6" max="6" width="31.109375" customWidth="1"/>
     <col min="7" max="7" width="38.21875" customWidth="1"/>
@@ -714,17 +713,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
+    <row r="7" spans="1:9"/>
     <row r="8" spans="1:9">
       <c r="A8" s="2">
         <v>6</v>
@@ -733,22 +722,22 @@
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -759,22 +748,22 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -785,25 +774,25 @@
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -814,30 +803,30 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -856,10 +845,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>12</v>
@@ -871,7 +860,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>31</v>
@@ -885,10 +874,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
@@ -900,7 +889,7 @@
         <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>31</v>
@@ -914,22 +903,22 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>31</v>
@@ -943,13 +932,13 @@
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
@@ -958,13 +947,13 @@
         <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -972,13 +961,13 @@
         <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>13</v>
@@ -987,13 +976,13 @@
         <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1001,28 +990,28 @@
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -1030,25 +1019,35 @@
         <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="D25" s="3"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed some API config
</commit_message>
<xml_diff>
--- a/04_API/APIs.xlsx
+++ b/04_API/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\github-for-aspire\capstone\04_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8602A2AE-3855-451D-86F1-F01AEB605DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBB381A-D747-49CF-AA23-9DDB79518A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
   <si>
     <t>Sr No</t>
   </si>
@@ -187,58 +187,58 @@
     <t>VOTE / COMMENT related APIs</t>
   </si>
   <si>
-    <t>/post/:title/upvote</t>
-  </si>
-  <si>
     <t>Upvotes / Unupvotes the post</t>
   </si>
   <si>
     <t>{"message": "Saved Successfully"}</t>
   </si>
   <si>
-    <t>/post/:title/downvote</t>
-  </si>
-  <si>
     <t>Downvotes / Un-downvotes the post</t>
   </si>
   <si>
-    <t>/post/:title/comment</t>
-  </si>
-  <si>
     <t>Adding a comment on a post</t>
   </si>
   <si>
     <t>comment_content, parent_type</t>
   </si>
   <si>
-    <t>/post/:post_title/:comment/upvote</t>
-  </si>
-  <si>
     <t>Upvotes / Unupvotes the comment</t>
   </si>
   <si>
-    <t>post_title, comment</t>
-  </si>
-  <si>
     <t>404: Post / Comment does not exist, 401: Unauthorized</t>
   </si>
   <si>
-    <t>/post/:post_title/:comment/downvote</t>
-  </si>
-  <si>
     <t>Downvotes / Un-downvotes the comment</t>
   </si>
   <si>
-    <t>/post/:post_title/:comment/reply</t>
-  </si>
-  <si>
     <t>Adding a comment on a comment</t>
   </si>
   <si>
-    <t>/post/:post_title/:comment</t>
-  </si>
-  <si>
     <t>Deleting a comment</t>
+  </si>
+  <si>
+    <t>/pages/upvote/:title</t>
+  </si>
+  <si>
+    <t>/pages/downvote/:title</t>
+  </si>
+  <si>
+    <t>/pages/comment/:title</t>
+  </si>
+  <si>
+    <t>comment_id</t>
+  </si>
+  <si>
+    <t>/pages/:title/comments/upvote</t>
+  </si>
+  <si>
+    <t>/pages/:title/comments/downvote</t>
+  </si>
+  <si>
+    <t>/pages/:title/comments/reply</t>
+  </si>
+  <si>
+    <t>/pages/:title/comments</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -539,7 +539,7 @@
     <col min="9" max="9" width="78.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="13.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="13.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -597,7 +597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="13.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -626,7 +626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="13.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -655,7 +655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="13.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -684,7 +684,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="13.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -713,8 +713,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9"/>
-    <row r="8" spans="1:9">
+    <row r="7" spans="1:9" ht="13.2"/>
+    <row r="8" spans="1:9" ht="13.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -740,7 +740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="13.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -766,7 +766,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="13.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -795,7 +795,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="13.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -824,7 +824,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="13.2">
       <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="13.2">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -845,10 +845,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>12</v>
@@ -860,13 +860,13 @@
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="13.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -874,10 +874,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
@@ -889,13 +889,13 @@
         <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="13.2">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -903,28 +903,28 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="13.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -932,28 +932,28 @@
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.2">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -961,28 +961,28 @@
         <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.2">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -990,28 +990,28 @@
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.2">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -1019,22 +1019,25 @@
         <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>65</v>
+        <v>12</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">

</xml_diff>